<commit_message>
lectures 11 and 12
</commit_message>
<xml_diff>
--- a/resources/lecture12.xlsx
+++ b/resources/lecture12.xlsx
@@ -38,22 +38,22 @@
     <t>Average Speed</t>
   </si>
   <si>
+    <t>Antwerp</t>
+  </si>
+  <si>
+    <t>Heusden-Zolder</t>
+  </si>
+  <si>
+    <t>Ghent</t>
+  </si>
+  <si>
     <t>Schulen</t>
   </si>
   <si>
     <t>Lummen</t>
   </si>
   <si>
-    <t>Antwerp</t>
-  </si>
-  <si>
     <t>Brussels</t>
-  </si>
-  <si>
-    <t>Ghent</t>
-  </si>
-  <si>
-    <t>Heusden-Zolder</t>
   </si>
 </sst>
 </file>
@@ -106,6 +106,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" ref="A1:H26" displayName="RUNNINGRESULTS" name="RUNNINGRESULTS">
+  <autoFilter ref="A1:H26"/>
   <tableColumns count="8">
     <tableColumn name="Start Date" id="1"/>
     <tableColumn name="Start Time" id="2"/>
@@ -128,14 +129,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="10.265625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.15625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.34765625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.30859375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="9.3046875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="8.921875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.35546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="12.0" customWidth="true"/>
+    <col min="2" max="2" width="12.0" customWidth="true"/>
+    <col min="3" max="3" width="12.0" customWidth="true"/>
+    <col min="4" max="4" width="12.0" customWidth="true"/>
+    <col min="5" max="5" width="12.0" customWidth="true"/>
+    <col min="6" max="6" width="12.0" customWidth="true"/>
+    <col min="7" max="7" width="12.0" customWidth="true"/>
+    <col min="8" max="8" width="12.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -166,22 +167,22 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>43102.09266959491</v>
+        <v>43101.4108352662</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>43102.09266959491</v>
+        <v>43101.4108352662</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43102.122067743054</v>
+        <v>43101.43955054398</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>43102.122067743054</v>
+        <v>43101.43955054398</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>8.357340627623513</v>
+        <v>8.516109537338451</v>
       </c>
       <c r="G2" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -192,22 +193,22 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>43110.40786559028</v>
+        <v>43107.17827626158</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43110.40786559028</v>
+        <v>43107.17827626158</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43110.428490590275</v>
+        <v>43107.20160959491</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>43110.428490590275</v>
+        <v>43107.20160959491</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>6.665689852353484</v>
+        <v>7.347180371568261</v>
       </c>
       <c r="G3" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -218,22 +219,22 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>43114.501507395835</v>
+        <v>43108.245410034724</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>43114.501507395835</v>
+        <v>43108.245410034724</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43114.54514165509</v>
+        <v>43108.26520170139</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>43114.54514165509</v>
+        <v>43108.26520170139</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>12.807348712798847</v>
+        <v>5.021017254063722</v>
       </c>
       <c r="G4" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -244,22 +245,22 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>43115.32139423611</v>
+        <v>43117.001220729166</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>43115.32139423611</v>
+        <v>43117.001220729166</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43115.353616458335</v>
+        <v>43117.021243877316</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>43115.353616458335</v>
+        <v>43117.021243877316</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>8.651589741666953</v>
+        <v>5.483717788175882</v>
       </c>
       <c r="G5" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -270,22 +271,22 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>43123.85141076389</v>
+        <v>43117.09622403935</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>43123.85141076389</v>
+        <v>43117.09622403935</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43123.88784594907</v>
+        <v>43117.14697635417</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>43123.88784594907</v>
+        <v>43117.14697635417</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>8.591198543522541</v>
+        <v>12.198801960702552</v>
       </c>
       <c r="G6" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -296,22 +297,22 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>43124.16337553241</v>
+        <v>43125.788834189814</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>43124.16337553241</v>
+        <v>43125.788834189814</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43124.19234543981</v>
+        <v>43125.806334189816</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>43124.19234543981</v>
+        <v>43125.806334189816</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>6.451263737448333</v>
+        <v>5.432378764660736</v>
       </c>
       <c r="G7" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -322,22 +323,22 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>43124.1960328125</v>
+        <v>43134.27033746528</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>43124.1960328125</v>
+        <v>43134.27033746528</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43124.21820873843</v>
+        <v>43134.30185366898</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>43124.21820873843</v>
+        <v>43134.30185366898</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>5.36988455846284</v>
+        <v>10.048111582066234</v>
       </c>
       <c r="G8" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -348,22 +349,22 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>43127.21373380787</v>
+        <v>43148.45178474537</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>43127.21373380787</v>
+        <v>43148.45178474537</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43127.25835186343</v>
+        <v>43148.49251391204</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>43127.25835186343</v>
+        <v>43148.49251391204</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>12.669337975744124</v>
+        <v>13.0071459362053</v>
       </c>
       <c r="G9" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -374,22 +375,22 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>43137.74394101852</v>
+        <v>43157.8351708912</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>43137.74394101852</v>
+        <v>43157.8351708912</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>43137.78151046296</v>
+        <v>43157.86160607639</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>43137.78151046296</v>
+        <v>43157.86160607639</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>10.479975488855693</v>
+        <v>7.150295247138457</v>
       </c>
       <c r="G10" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -400,22 +401,22 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>43145.35080704861</v>
+        <v>43161.91693673611</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>43145.35080704861</v>
+        <v>43161.91693673611</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43145.38824917824</v>
+        <v>43161.951716828706</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>43145.38824917824</v>
+        <v>43161.951716828706</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>11.377372638928662</v>
+        <v>9.811889009469633</v>
       </c>
       <c r="G11" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -426,22 +427,22 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>43145.95556236111</v>
+        <v>43162.55858101852</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>43145.95556236111</v>
+        <v>43162.55858101852</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43145.998722083335</v>
+        <v>43162.59043287037</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>43145.998722083335</v>
+        <v>43162.59043287037</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>10.238929746915698</v>
+        <v>10.078978434153257</v>
       </c>
       <c r="G12" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -452,22 +453,22 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>43153.11574675926</v>
+        <v>43163.06331835648</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>43153.11574675926</v>
+        <v>43163.06331835648</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43153.15178842592</v>
+        <v>43163.09145493055</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>43153.15178842592</v>
+        <v>43163.09145493055</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>9.166553654541651</v>
+        <v>9.111168021047215</v>
       </c>
       <c r="G13" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -478,22 +479,22 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>43157.262369375</v>
+        <v>43171.775890046294</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>43157.262369375</v>
+        <v>43171.775890046294</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43157.291755949074</v>
+        <v>43171.799686342594</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>43157.291755949074</v>
+        <v>43171.799686342594</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>9.310830250313208</v>
+        <v>7.639479810321195</v>
       </c>
       <c r="G14" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -504,22 +505,22 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>43158.0468150463</v>
+        <v>43174.887463541665</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>43158.0468150463</v>
+        <v>43174.887463541665</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43158.06588912037</v>
+        <v>43174.90484780093</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>43158.06588912037</v>
+        <v>43174.90484780093</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>5.710092718952668</v>
+        <v>5.102015479309499</v>
       </c>
       <c r="G15" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -530,22 +531,22 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>43161.836449201386</v>
+        <v>43178.86926556713</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>43161.836449201386</v>
+        <v>43178.86926556713</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43161.89016447917</v>
+        <v>43178.89737899305</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>43161.89016447917</v>
+        <v>43178.89737899305</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>13.910545114925107</v>
+        <v>6.701229977060974</v>
       </c>
       <c r="G16" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -556,22 +557,22 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>43166.47065991898</v>
+        <v>43181.19306818287</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>43166.47065991898</v>
+        <v>43181.19306818287</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43166.50715297454</v>
+        <v>43181.235487164355</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>43166.50715297454</v>
+        <v>43181.235487164355</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>12.188131833557447</v>
+        <v>12.59215310002132</v>
       </c>
       <c r="G17" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -582,22 +583,22 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>43170.37540172454</v>
+        <v>43181.70130883102</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>43170.37540172454</v>
+        <v>43181.70130883102</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43170.40537857639</v>
+        <v>43181.73355420139</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>43170.40537857639</v>
+        <v>43181.73355420139</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>8.507362660721608</v>
+        <v>8.432484678444226</v>
       </c>
       <c r="G18" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -608,22 +609,22 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>43172.74351119213</v>
+        <v>43186.534220092595</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>43172.74351119213</v>
+        <v>43186.534220092595</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43172.7679903588</v>
+        <v>43186.56221777778</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>43172.7679903588</v>
+        <v>43186.56221777778</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>8.053355321792278</v>
+        <v>7.902374773276685</v>
       </c>
       <c r="G19" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -634,22 +635,22 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>43178.65641350694</v>
+        <v>43186.99159445602</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>43178.65641350694</v>
+        <v>43186.99159445602</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43178.70520980324</v>
+        <v>43187.04036760417</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>43178.70520980324</v>
+        <v>43187.04036760417</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>11.403309628202582</v>
+        <v>11.554691117278642</v>
       </c>
       <c r="G20" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -660,22 +661,22 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>43189.51742195602</v>
+        <v>43196.38063280092</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>43189.51742195602</v>
+        <v>43196.38063280092</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43189.54820899305</v>
+        <v>43196.402322615744</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>43189.54820899305</v>
+        <v>43196.402322615744</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F21" s="3" t="n">
-        <v>8.67741350840665</v>
+        <v>5.2430426184446315</v>
       </c>
       <c r="G21" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -686,22 +687,22 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>43192.54122561343</v>
+        <v>43200.46987519676</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>43192.54122561343</v>
+        <v>43200.46987519676</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43192.56090153935</v>
+        <v>43200.48728260417</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>43192.56090153935</v>
+        <v>43200.48728260417</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3" t="n">
-        <v>6.535217330932544</v>
+        <v>5.005267193320042</v>
       </c>
       <c r="G22" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -712,22 +713,22 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>43196.58627788194</v>
+        <v>43206.94643818287</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>43196.58627788194</v>
+        <v>43206.94643818287</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43196.604090381945</v>
+        <v>43206.99643818287</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>43196.604090381945</v>
+        <v>43206.99643818287</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F23" s="3" t="n">
-        <v>5.826875559023212</v>
+        <v>12.52107801286148</v>
       </c>
       <c r="G23" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -738,22 +739,22 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>43207.450856574076</v>
+        <v>43209.32189533565</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>43207.450856574076</v>
+        <v>43209.32189533565</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43207.483217685185</v>
+        <v>43209.353585150464</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>43207.483217685185</v>
+        <v>43209.353585150464</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>7.260293556816961</v>
+        <v>9.831140704045616</v>
       </c>
       <c r="G24" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -764,22 +765,22 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>43210.54441055556</v>
+        <v>43209.38638125</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>43210.54441055556</v>
+        <v>43209.38638125</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>43210.572165185185</v>
+        <v>43209.40896226852</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>43210.572165185185</v>
+        <v>43209.40896226852</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3" t="n">
-        <v>7.112527042257852</v>
+        <v>6.996415265612087</v>
       </c>
       <c r="G25" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -790,22 +791,22 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>43219.097647152776</v>
+        <v>43215.25432825232</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>43219.097647152776</v>
+        <v>43215.25432825232</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>43219.13206844907</v>
+        <v>43215.29827501158</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>43219.13206844907</v>
+        <v>43215.29827501158</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" s="3" t="n">
-        <v>10.87164232333646</v>
+        <v>11.444874747463466</v>
       </c>
       <c r="G26" s="2">
         <f>INDIRECT("C"&amp;ROW())-INDIRECT("B"&amp;ROW())</f>
@@ -815,38 +816,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H27">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50.0"/>
-        <cfvo type="max"/>
-        <color rgb="FF0000"/>
-        <color rgb="FF9900"/>
-        <color rgb="006600"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F27">
-    <cfRule type="iconSet" priority="2">
-      <iconSet iconSet="5Rating">
-        <cfvo type="percentile" val="0.0"/>
-        <cfvo type="percentile" val="25.0"/>
-        <cfvo type="percentile" val="50.0"/>
-        <cfvo type="percentile" val="75.0"/>
-        <cfvo type="percentile" val="100.0"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
-    <cfRule type="dataBar" priority="3">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="006600"/>
-      </dataBar>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts>
     <tablePart r:id="rId1"/>

</xml_diff>